<commit_message>
wip: adicionado dados ao projeto.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath\Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A8DF5D-FC94-4D42-98B7-A4E2FE7F5E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34D59D4-738A-4273-859A-AFFB7704080F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>